<commit_message>
Enable parallel execution with Docker Grid and thread-safe TestNG framework
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aniket\eclipse-workspace\opencart\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aniket\git\aniket5889\opencart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,17 +441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -473,7 +473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -484,7 +484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -495,7 +495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -506,7 +506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>

</xml_diff>